<commit_message>
Added informative warning wen type_stat misspelt
</commit_message>
<xml_diff>
--- a/fake_test_data_0001.xlsx
+++ b/fake_test_data_0001.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t xml:space="preserve">Coder: </t>
   </si>
@@ -168,7 +168,19 @@
     <t>npv</t>
   </si>
   <si>
-    <t>accu</t>
+    <t>accurac</t>
+  </si>
+  <si>
+    <t>accucc</t>
+  </si>
+  <si>
+    <t>senss</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>specif</t>
   </si>
 </sst>
 </file>
@@ -224,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -235,11 +247,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,8 +473,8 @@
   </sheetPr>
   <dimension ref="A1:AJ1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -474,27 +487,27 @@
         <v>42</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="10" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
       <c r="Q1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1092,7 +1105,7 @@
       <c r="B14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>92</v>
       </c>
       <c r="F14" s="9">
@@ -1135,7 +1148,7 @@
       <c r="B15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>96</v>
       </c>
       <c r="F15" s="9">
@@ -1178,7 +1191,7 @@
       <c r="B16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>71</v>
       </c>
       <c r="F16" s="9">
@@ -1221,7 +1234,7 @@
       <c r="B17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>87</v>
       </c>
       <c r="F17" s="9">
@@ -1264,7 +1277,7 @@
       <c r="B18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>86</v>
       </c>
       <c r="F18" s="9">
@@ -1305,9 +1318,9 @@
         <v>10</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>96</v>
       </c>
       <c r="F19" s="9">
@@ -1344,6 +1357,29 @@
       <c r="AJ19" s="7"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>11</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="10">
+        <v>90</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10">
+        <v>90</v>
+      </c>
+      <c r="G20" s="10">
+        <v>24</v>
+      </c>
+      <c r="H20" s="10">
+        <v>8</v>
+      </c>
+      <c r="I20" s="10">
+        <v>10</v>
+      </c>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
@@ -1366,6 +1402,29 @@
       <c r="AJ20" s="7"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>11</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="10">
+        <v>92</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10">
+        <v>90</v>
+      </c>
+      <c r="G21" s="10">
+        <v>24</v>
+      </c>
+      <c r="H21" s="10">
+        <v>8</v>
+      </c>
+      <c r="I21" s="10">
+        <v>10</v>
+      </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
@@ -1388,6 +1447,29 @@
       <c r="AJ21" s="7"/>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>22</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="10">
+        <v>75</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10">
+        <v>90</v>
+      </c>
+      <c r="G22" s="10">
+        <v>24</v>
+      </c>
+      <c r="H22" s="10">
+        <v>8</v>
+      </c>
+      <c r="I22" s="10">
+        <v>10</v>
+      </c>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>

</xml_diff>

<commit_message>
Added robustness when rounding values ending in 5
</commit_message>
<xml_diff>
--- a/fake_test_data_0001.xlsx
+++ b/fake_test_data_0001.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t xml:space="preserve">Coder: </t>
   </si>
@@ -182,6 +182,9 @@
   <si>
     <t>specif</t>
   </si>
+  <si>
+    <t>accu</t>
+  </si>
 </sst>
 </file>
 
@@ -236,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -249,6 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,10 +475,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ1002"/>
+  <dimension ref="A1:AJ1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -487,27 +491,27 @@
         <v>42</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="12" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="12" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
       <c r="Q1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1270,26 +1274,26 @@
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
+    <row r="18" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12">
+        <v>11</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>49</v>
+      <c r="B18" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="C18" s="11">
         <v>86</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="12">
         <v>90</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="12">
         <v>24</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="12">
         <v>8</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="12">
         <v>10</v>
       </c>
       <c r="Q18" s="7"/>
@@ -1313,26 +1317,26 @@
       <c r="AI18" s="7"/>
       <c r="AJ18" s="7"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
-        <v>10</v>
+    <row r="19" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12">
+        <v>11</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>50</v>
+      <c r="B19" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="11">
-        <v>96</v>
+        <v>85</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="12">
         <v>90</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="12">
         <v>24</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="12">
         <v>8</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="12">
         <v>10</v>
       </c>
       <c r="Q19" s="7"/>
@@ -1357,27 +1361,25 @@
       <c r="AJ19" s="7"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
-        <v>11</v>
+      <c r="A20" s="9">
+        <v>12</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>51</v>
+      <c r="B20" s="9" t="s">
+        <v>49</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="11">
+        <v>86</v>
+      </c>
+      <c r="F20" s="9">
         <v>90</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10">
-        <v>90</v>
-      </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <v>24</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="9">
         <v>8</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <v>10</v>
       </c>
       <c r="Q20" s="7"/>
@@ -1402,27 +1404,25 @@
       <c r="AJ20" s="7"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
-        <v>11</v>
+      <c r="A21" s="9">
+        <v>12</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>52</v>
+      <c r="B21" s="9" t="s">
+        <v>50</v>
       </c>
-      <c r="C21" s="10">
-        <v>92</v>
+      <c r="C21" s="11">
+        <v>96</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>90</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <v>24</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="9">
         <v>8</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="9">
         <v>10</v>
       </c>
       <c r="Q21" s="7"/>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="10">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -1492,6 +1492,29 @@
       <c r="AJ22" s="7"/>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>13</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="10">
+        <v>92</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10">
+        <v>90</v>
+      </c>
+      <c r="G23" s="10">
+        <v>24</v>
+      </c>
+      <c r="H23" s="10">
+        <v>8</v>
+      </c>
+      <c r="I23" s="10">
+        <v>10</v>
+      </c>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
@@ -1514,6 +1537,29 @@
       <c r="AJ23" s="7"/>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="10">
+        <v>75</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10">
+        <v>90</v>
+      </c>
+      <c r="G24" s="10">
+        <v>24</v>
+      </c>
+      <c r="H24" s="10">
+        <v>8</v>
+      </c>
+      <c r="I24" s="10">
+        <v>10</v>
+      </c>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
@@ -23051,6 +23097,50 @@
       <c r="AI1002" s="7"/>
       <c r="AJ1002" s="7"/>
     </row>
+    <row r="1003" spans="17:36" x14ac:dyDescent="0.2">
+      <c r="Q1003" s="7"/>
+      <c r="R1003" s="7"/>
+      <c r="S1003" s="7"/>
+      <c r="T1003" s="7"/>
+      <c r="U1003" s="7"/>
+      <c r="V1003" s="7"/>
+      <c r="W1003" s="7"/>
+      <c r="X1003" s="7"/>
+      <c r="Y1003" s="7"/>
+      <c r="Z1003" s="7"/>
+      <c r="AA1003" s="7"/>
+      <c r="AB1003" s="7"/>
+      <c r="AC1003" s="7"/>
+      <c r="AD1003" s="7"/>
+      <c r="AE1003" s="7"/>
+      <c r="AF1003" s="7"/>
+      <c r="AG1003" s="7"/>
+      <c r="AH1003" s="7"/>
+      <c r="AI1003" s="7"/>
+      <c r="AJ1003" s="7"/>
+    </row>
+    <row r="1004" spans="17:36" x14ac:dyDescent="0.2">
+      <c r="Q1004" s="7"/>
+      <c r="R1004" s="7"/>
+      <c r="S1004" s="7"/>
+      <c r="T1004" s="7"/>
+      <c r="U1004" s="7"/>
+      <c r="V1004" s="7"/>
+      <c r="W1004" s="7"/>
+      <c r="X1004" s="7"/>
+      <c r="Y1004" s="7"/>
+      <c r="Z1004" s="7"/>
+      <c r="AA1004" s="7"/>
+      <c r="AB1004" s="7"/>
+      <c r="AC1004" s="7"/>
+      <c r="AD1004" s="7"/>
+      <c r="AE1004" s="7"/>
+      <c r="AF1004" s="7"/>
+      <c r="AG1004" s="7"/>
+      <c r="AH1004" s="7"/>
+      <c r="AI1004" s="7"/>
+      <c r="AJ1004" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="M1:P1"/>

</xml_diff>

<commit_message>
added tests for ratios + changed template from a-d to n11-n22
</commit_message>
<xml_diff>
--- a/fake_test_data_0001.xlsx
+++ b/fake_test_data_0001.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t xml:space="preserve">Coder: </t>
   </si>
@@ -73,18 +73,6 @@
   </si>
   <si>
     <t>df2</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
   <si>
     <t>value1</t>
@@ -185,6 +173,27 @@
   <si>
     <t>accu</t>
   </si>
+  <si>
+    <t>risk_ratio</t>
+  </si>
+  <si>
+    <t>risk_diff</t>
+  </si>
+  <si>
+    <t>odds_ratio</t>
+  </si>
+  <si>
+    <t>n11</t>
+  </si>
+  <si>
+    <t>n12</t>
+  </si>
+  <si>
+    <t>n22</t>
+  </si>
+  <si>
+    <t>n21</t>
+  </si>
 </sst>
 </file>
 
@@ -239,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -252,6 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,8 +487,8 @@
   </sheetPr>
   <dimension ref="A1:AJ1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -488,30 +498,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="13" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="13" t="s">
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
       <c r="Q1" s="3" t="s">
         <v>6</v>
       </c>
@@ -573,76 +583,76 @@
         <v>17</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="R2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="S2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="T2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="AG2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
@@ -650,7 +660,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>168</v>
@@ -689,7 +699,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>40</v>
@@ -726,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>1003</v>
@@ -787,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>120</v>
@@ -826,7 +836,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>108</v>
@@ -935,7 +945,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C10" s="9">
         <v>90</v>
@@ -978,7 +988,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C11" s="9">
         <v>92</v>
@@ -1021,7 +1031,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C12" s="9">
         <v>75</v>
@@ -1064,7 +1074,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C13" s="9">
         <v>85</v>
@@ -1107,7 +1117,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" s="11">
         <v>92</v>
@@ -1150,7 +1160,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C15" s="11">
         <v>96</v>
@@ -1193,7 +1203,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C16" s="11">
         <v>71</v>
@@ -1236,7 +1246,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C17" s="11">
         <v>87</v>
@@ -1279,7 +1289,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C18" s="11">
         <v>86</v>
@@ -1322,7 +1332,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C19" s="11">
         <v>85</v>
@@ -1365,7 +1375,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C20" s="11">
         <v>86</v>
@@ -1408,7 +1418,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C21" s="11">
         <v>96</v>
@@ -1451,7 +1461,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C22" s="10">
         <v>90</v>
@@ -1496,7 +1506,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C23" s="10">
         <v>92</v>
@@ -1541,7 +1551,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C24" s="10">
         <v>75</v>
@@ -1582,6 +1592,27 @@
       <c r="AJ24" s="7"/>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
+        <v>18</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M25">
+        <v>13</v>
+      </c>
+      <c r="N25">
+        <v>32</v>
+      </c>
+      <c r="O25">
+        <v>17</v>
+      </c>
+      <c r="P25">
+        <v>23</v>
+      </c>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
@@ -1604,6 +1635,27 @@
       <c r="AJ25" s="7"/>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
+        <v>18</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="13">
+        <v>1.55</v>
+      </c>
+      <c r="M26" s="13">
+        <v>13</v>
+      </c>
+      <c r="N26" s="13">
+        <v>32</v>
+      </c>
+      <c r="O26" s="13">
+        <v>17</v>
+      </c>
+      <c r="P26" s="13">
+        <v>23</v>
+      </c>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
       <c r="S26" s="7"/>
@@ -1626,6 +1678,27 @@
       <c r="AJ26" s="7"/>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A27" s="13">
+        <v>25</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="13">
+        <v>0.68</v>
+      </c>
+      <c r="M27" s="13">
+        <v>13</v>
+      </c>
+      <c r="N27" s="13">
+        <v>32</v>
+      </c>
+      <c r="O27" s="13">
+        <v>17</v>
+      </c>
+      <c r="P27" s="13">
+        <v>23</v>
+      </c>
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
       <c r="S27" s="7"/>
@@ -1648,6 +1721,27 @@
       <c r="AJ27" s="7"/>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A28" s="13">
+        <v>25</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="13">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="M28" s="13">
+        <v>13</v>
+      </c>
+      <c r="N28" s="13">
+        <v>32</v>
+      </c>
+      <c r="O28" s="13">
+        <v>17</v>
+      </c>
+      <c r="P28" s="13">
+        <v>23</v>
+      </c>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>
@@ -1670,6 +1764,27 @@
       <c r="AJ28" s="7"/>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A29" s="13">
+        <v>27</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="13">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="M29" s="13">
+        <v>13</v>
+      </c>
+      <c r="N29" s="13">
+        <v>32</v>
+      </c>
+      <c r="O29" s="13">
+        <v>17</v>
+      </c>
+      <c r="P29" s="13">
+        <v>23</v>
+      </c>
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
@@ -1692,6 +1807,27 @@
       <c r="AJ29" s="7"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A30" s="13">
+        <v>27</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M30" s="13">
+        <v>13</v>
+      </c>
+      <c r="N30" s="13">
+        <v>32</v>
+      </c>
+      <c r="O30" s="13">
+        <v>17</v>
+      </c>
+      <c r="P30" s="13">
+        <v>23</v>
+      </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
       <c r="S30" s="7"/>

</xml_diff>

<commit_message>
Change so coders always fill in df1
</commit_message>
<xml_diff>
--- a/fake_test_data_0001.xlsx
+++ b/fake_test_data_0001.xlsx
@@ -518,16 +518,17 @@
   </sheetPr>
   <dimension ref="A1:AK1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.42578125" style="3"/>
-    <col min="3" max="3" width="14.42578125" style="6"/>
-    <col min="4" max="4" width="14.42578125" style="7"/>
-    <col min="5" max="16384" width="14.42578125" style="3"/>
+    <col min="3" max="3" width="14.42578125" style="7"/>
+    <col min="4" max="9" width="14.42578125" style="3"/>
+    <col min="10" max="10" width="14.42578125" style="6"/>
+    <col min="11" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
@@ -538,17 +539,17 @@
         <v>38</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="J1" s="1"/>
       <c r="K1" s="9" t="s">
         <v>3</v>
       </c>
@@ -591,28 +592,28 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>4</v>
@@ -703,7 +704,7 @@
       <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="7">
+      <c r="C3" s="7">
         <v>168</v>
       </c>
       <c r="R3" s="2">
@@ -742,7 +743,7 @@
       <c r="B4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="7">
+      <c r="C4" s="7">
         <v>40</v>
       </c>
       <c r="R4" s="2">
@@ -779,7 +780,7 @@
       <c r="B5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="7">
+      <c r="C5" s="7">
         <v>1003</v>
       </c>
       <c r="R5" s="2">
@@ -840,7 +841,7 @@
       <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="7">
+      <c r="C6" s="7">
         <v>120</v>
       </c>
       <c r="R6" s="2">
@@ -879,7 +880,7 @@
       <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="7">
+      <c r="C7" s="7">
         <v>108</v>
       </c>
       <c r="R7" s="2">
@@ -914,13 +915,13 @@
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="7">
+      <c r="C8" s="7">
         <v>25</v>
       </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
       <c r="E8" s="3">
-        <v>4</v>
-      </c>
-      <c r="F8" s="3">
         <v>16</v>
       </c>
       <c r="R8" s="2"/>
@@ -951,13 +952,13 @@
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="7">
+      <c r="C9" s="7">
         <v>32</v>
       </c>
+      <c r="D9" s="3">
+        <v>16</v>
+      </c>
       <c r="E9" s="3">
-        <v>16</v>
-      </c>
-      <c r="F9" s="3">
         <v>48</v>
       </c>
       <c r="R9" s="2"/>
@@ -988,19 +989,19 @@
       <c r="B10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="7">
+      <c r="C10" s="7">
         <v>90</v>
       </c>
+      <c r="F10" s="3">
+        <v>90</v>
+      </c>
       <c r="G10" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H10" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I10" s="3">
-        <v>8</v>
-      </c>
-      <c r="J10" s="3">
         <v>10</v>
       </c>
       <c r="R10" s="2"/>
@@ -1031,19 +1032,19 @@
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="7">
+      <c r="C11" s="7">
         <v>92</v>
       </c>
+      <c r="F11" s="3">
+        <v>90</v>
+      </c>
       <c r="G11" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H11" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I11" s="3">
-        <v>8</v>
-      </c>
-      <c r="J11" s="3">
         <v>10</v>
       </c>
       <c r="R11" s="2"/>
@@ -1074,19 +1075,19 @@
       <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="7">
+      <c r="C12" s="7">
         <v>75</v>
       </c>
+      <c r="F12" s="3">
+        <v>90</v>
+      </c>
       <c r="G12" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H12" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I12" s="3">
-        <v>8</v>
-      </c>
-      <c r="J12" s="3">
         <v>10</v>
       </c>
       <c r="R12" s="2"/>
@@ -1117,19 +1118,19 @@
       <c r="B13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="7">
+      <c r="C13" s="7">
         <v>85</v>
       </c>
+      <c r="F13" s="3">
+        <v>90</v>
+      </c>
       <c r="G13" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H13" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I13" s="3">
-        <v>8</v>
-      </c>
-      <c r="J13" s="3">
         <v>10</v>
       </c>
       <c r="R13" s="2"/>
@@ -1160,22 +1161,22 @@
       <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
+      <c r="C14" s="4">
         <v>92</v>
       </c>
+      <c r="F14" s="3">
+        <v>90</v>
+      </c>
       <c r="G14" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H14" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I14" s="3">
-        <v>8</v>
-      </c>
-      <c r="J14" s="3">
         <v>10</v>
       </c>
+      <c r="J14" s="4"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
@@ -1204,22 +1205,22 @@
       <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4">
+      <c r="C15" s="4">
         <v>96</v>
       </c>
+      <c r="F15" s="3">
+        <v>90</v>
+      </c>
       <c r="G15" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H15" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I15" s="3">
-        <v>8</v>
-      </c>
-      <c r="J15" s="3">
         <v>10</v>
       </c>
+      <c r="J15" s="4"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
@@ -1248,22 +1249,22 @@
       <c r="B16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4">
+      <c r="C16" s="4">
         <v>71</v>
       </c>
+      <c r="F16" s="3">
+        <v>90</v>
+      </c>
       <c r="G16" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H16" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I16" s="3">
-        <v>8</v>
-      </c>
-      <c r="J16" s="3">
         <v>10</v>
       </c>
+      <c r="J16" s="4"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
@@ -1292,22 +1293,22 @@
       <c r="B17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4">
+      <c r="C17" s="4">
         <v>87</v>
       </c>
+      <c r="F17" s="3">
+        <v>90</v>
+      </c>
       <c r="G17" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H17" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I17" s="3">
-        <v>8</v>
-      </c>
-      <c r="J17" s="3">
         <v>10</v>
       </c>
+      <c r="J17" s="4"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
@@ -1336,22 +1337,22 @@
       <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4">
+      <c r="C18" s="4">
         <v>86</v>
       </c>
+      <c r="F18" s="3">
+        <v>90</v>
+      </c>
       <c r="G18" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H18" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I18" s="3">
-        <v>8</v>
-      </c>
-      <c r="J18" s="3">
         <v>10</v>
       </c>
+      <c r="J18" s="4"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
@@ -1380,22 +1381,22 @@
       <c r="B19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4">
+      <c r="C19" s="4">
         <v>85</v>
       </c>
+      <c r="F19" s="3">
+        <v>90</v>
+      </c>
       <c r="G19" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H19" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I19" s="3">
-        <v>8</v>
-      </c>
-      <c r="J19" s="3">
         <v>10</v>
       </c>
+      <c r="J19" s="4"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
@@ -1424,22 +1425,22 @@
       <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4">
+      <c r="C20" s="4">
         <v>86</v>
       </c>
+      <c r="F20" s="3">
+        <v>90</v>
+      </c>
       <c r="G20" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H20" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I20" s="3">
-        <v>8</v>
-      </c>
-      <c r="J20" s="3">
         <v>10</v>
       </c>
+      <c r="J20" s="4"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
@@ -1468,22 +1469,22 @@
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4">
+      <c r="C21" s="4">
         <v>96</v>
       </c>
+      <c r="F21" s="3">
+        <v>90</v>
+      </c>
       <c r="G21" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H21" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I21" s="3">
-        <v>8</v>
-      </c>
-      <c r="J21" s="3">
         <v>10</v>
       </c>
+      <c r="J21" s="4"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
@@ -1512,19 +1513,19 @@
       <c r="B22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="7">
+      <c r="C22" s="7">
         <v>90</v>
       </c>
+      <c r="F22" s="3">
+        <v>90</v>
+      </c>
       <c r="G22" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H22" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I22" s="3">
-        <v>8</v>
-      </c>
-      <c r="J22" s="3">
         <v>10</v>
       </c>
       <c r="R22" s="2"/>
@@ -1555,19 +1556,19 @@
       <c r="B23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="7">
+      <c r="C23" s="7">
         <v>92</v>
       </c>
+      <c r="F23" s="3">
+        <v>90</v>
+      </c>
       <c r="G23" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H23" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I23" s="3">
-        <v>8</v>
-      </c>
-      <c r="J23" s="3">
         <v>10</v>
       </c>
       <c r="R23" s="2"/>
@@ -1598,19 +1599,19 @@
       <c r="B24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="7">
+      <c r="C24" s="7">
         <v>75</v>
       </c>
+      <c r="F24" s="3">
+        <v>90</v>
+      </c>
       <c r="G24" s="3">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H24" s="3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I24" s="3">
-        <v>8</v>
-      </c>
-      <c r="J24" s="3">
         <v>10</v>
       </c>
       <c r="R24" s="2"/>
@@ -1641,7 +1642,7 @@
       <c r="B25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="7">
+      <c r="C25" s="7">
         <v>0.55000000000000004</v>
       </c>
       <c r="N25" s="3">
@@ -1684,7 +1685,7 @@
       <c r="B26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="7">
+      <c r="C26" s="7">
         <v>1.55</v>
       </c>
       <c r="N26" s="3">
@@ -1727,7 +1728,7 @@
       <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="7">
+      <c r="C27" s="7">
         <v>0.68</v>
       </c>
       <c r="N27" s="3">
@@ -1770,7 +1771,7 @@
       <c r="B28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="7">
+      <c r="C28" s="7">
         <v>0.67900000000000005</v>
       </c>
       <c r="N28" s="3">
@@ -1813,7 +1814,7 @@
       <c r="B29" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="7">
+      <c r="C29" s="7">
         <v>-0.14000000000000001</v>
       </c>
       <c r="N29" s="3">
@@ -1856,7 +1857,7 @@
       <c r="B30" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="7">
+      <c r="C30" s="7">
         <v>0.14000000000000001</v>
       </c>
       <c r="N30" s="3">
@@ -1899,13 +1900,13 @@
       <c r="B31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="7">
+      <c r="C31" s="7">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="K31" s="3">
         <v>1.92</v>
       </c>
-      <c r="M31" s="3">
+      <c r="L31" s="3">
         <v>32</v>
       </c>
       <c r="R31" s="2"/>
@@ -1936,13 +1937,13 @@
       <c r="B32" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="7">
+      <c r="C32" s="7">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="K32" s="3">
         <v>1.92</v>
       </c>
-      <c r="M32" s="3">
+      <c r="L32" s="3">
         <v>32</v>
       </c>
       <c r="R32" s="2"/>
@@ -1973,13 +1974,13 @@
       <c r="B33" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="7">
+      <c r="C33" s="7">
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="K33" s="3">
         <v>1.92</v>
       </c>
-      <c r="M33" s="3">
+      <c r="L33" s="3">
         <v>32</v>
       </c>
       <c r="R33" s="2"/>
@@ -2010,7 +2011,7 @@
       <c r="B34" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="7">
+      <c r="C34" s="7">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="K34" s="3">
@@ -2050,7 +2051,7 @@
       <c r="B35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="7">
+      <c r="C35" s="7">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="K35" s="3">
@@ -2090,7 +2091,7 @@
       <c r="B36" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="7">
+      <c r="C36" s="7">
         <v>1E-3</v>
       </c>
       <c r="K36" s="3">
@@ -2124,7 +2125,7 @@
       <c r="B37" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="7">
+      <c r="C37" s="7">
         <v>0.01</v>
       </c>
       <c r="K37" s="3">
@@ -2158,14 +2159,14 @@
       <c r="B38" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4">
+      <c r="C38" s="4">
         <v>0.01</v>
       </c>
+      <c r="J38" s="4"/>
       <c r="K38" s="3">
         <v>0.32</v>
       </c>
-      <c r="M38" s="3">
+      <c r="L38" s="3">
         <v>50</v>
       </c>
       <c r="R38" s="2"/>
@@ -2196,14 +2197,14 @@
       <c r="B39" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4">
+      <c r="C39" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
+      <c r="J39" s="4"/>
       <c r="K39" s="3">
         <v>0.15</v>
       </c>
-      <c r="M39" s="3">
+      <c r="L39" s="3">
         <v>250</v>
       </c>
       <c r="R39" s="2"/>
@@ -2234,10 +2235,10 @@
       <c r="B40" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4">
+      <c r="C40" s="4">
         <v>0.16</v>
       </c>
+      <c r="J40" s="4"/>
       <c r="K40" s="4">
         <v>5.23</v>
       </c>
@@ -2272,10 +2273,10 @@
       <c r="B41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4">
+      <c r="C41" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="J41" s="4"/>
       <c r="K41" s="4">
         <v>5.23</v>
       </c>
@@ -2310,10 +2311,10 @@
       <c r="B42" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4">
+      <c r="C42" s="4">
         <v>8.9399999999999993E-2</v>
       </c>
+      <c r="J42" s="4"/>
       <c r="K42" s="4">
         <v>13.72</v>
       </c>
@@ -2348,10 +2349,10 @@
       <c r="B43" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4">
+      <c r="C43" s="4">
         <v>8.9300000000000004E-2</v>
       </c>
+      <c r="J43" s="4"/>
       <c r="K43" s="4">
         <v>13.72</v>
       </c>
@@ -2386,18 +2387,18 @@
       <c r="B44" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="8">
+      <c r="C44" s="8">
         <v>0.68</v>
       </c>
+      <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
+      <c r="J44" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
@@ -2441,18 +2442,18 @@
       <c r="B45" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="4">
+      <c r="C45" s="4">
         <v>0.16</v>
       </c>
+      <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
+      <c r="J45" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="K45" s="4">
         <v>13.72</v>
       </c>
@@ -2487,18 +2488,18 @@
       <c r="B46" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46" s="4">
+      <c r="C46" s="4">
         <v>0.01</v>
       </c>
+      <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
+      <c r="J46" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="K46" s="6">
         <v>2.83</v>
       </c>
@@ -2573,7 +2574,7 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
     </row>
-    <row r="49" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R49" s="2"/>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
@@ -2595,8 +2596,8 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
     </row>
-    <row r="50" spans="4:37" x14ac:dyDescent="0.2">
-      <c r="D50" s="4"/>
+    <row r="50" spans="3:37" x14ac:dyDescent="0.2">
+      <c r="C50" s="4"/>
       <c r="R50" s="2"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
@@ -2618,8 +2619,8 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
     </row>
-    <row r="51" spans="4:37" x14ac:dyDescent="0.2">
-      <c r="D51" s="4"/>
+    <row r="51" spans="3:37" x14ac:dyDescent="0.2">
+      <c r="C51" s="4"/>
       <c r="R51" s="2"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
@@ -2641,7 +2642,7 @@
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R52" s="2"/>
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
@@ -2663,7 +2664,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="53" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R53" s="2"/>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
@@ -2685,7 +2686,7 @@
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
     </row>
-    <row r="54" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
@@ -2707,7 +2708,7 @@
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
@@ -2729,7 +2730,7 @@
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
     </row>
-    <row r="56" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
@@ -2751,7 +2752,7 @@
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
@@ -2773,7 +2774,7 @@
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
     </row>
-    <row r="58" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
@@ -2795,7 +2796,7 @@
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
     </row>
-    <row r="59" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
@@ -2817,7 +2818,7 @@
       <c r="AJ59" s="2"/>
       <c r="AK59" s="2"/>
     </row>
-    <row r="60" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
@@ -2839,7 +2840,7 @@
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
     </row>
-    <row r="61" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
@@ -2861,7 +2862,7 @@
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
     </row>
-    <row r="62" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
@@ -2883,7 +2884,7 @@
       <c r="AJ62" s="2"/>
       <c r="AK62" s="2"/>
     </row>
-    <row r="63" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
@@ -2905,7 +2906,7 @@
       <c r="AJ63" s="2"/>
       <c r="AK63" s="2"/>
     </row>
-    <row r="64" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:37" x14ac:dyDescent="0.2">
       <c r="R64" s="2"/>
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
@@ -23610,8 +23611,8 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>